<commit_message>
fix(Import): reliable detection of intented datetime type
Signed-off-by: Arthur Schiwon <blizzz@arthur-schiwon.de>
</commit_message>
<xml_diff>
--- a/tests/integration/resources/import-from-libreoffice.xlsx
+++ b/tests/integration/resources/import-from-libreoffice.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t xml:space="preserve">Date and Time</t>
+  </si>
   <si>
     <t xml:space="preserve">Col1</t>
   </si>
@@ -44,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">truth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time</t>
   </si>
   <si>
     <t xml:space="preserve">Val1</t>
@@ -80,17 +86,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="167" formatCode="General"/>
+    <numFmt numFmtId="168" formatCode="hh:mm"/>
   </numFmts>
   <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -112,21 +119,18 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="13.5"/>
       <color rgb="FF5C92FF"/>
       <name val="Noto Sans"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="13.5"/>
       <color rgb="FF5C92FF"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -171,7 +175,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -180,6 +184,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -188,11 +200,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -383,13 +399,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="B:H"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.25"/>
+  </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -416,63 +435,80 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0"/>
-      <c r="J1" s="0"/>
-      <c r="K1" s="0"/>
-      <c r="L1" s="0"/>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="3" t="n">
+        <v>44612.3625</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="4" t="n">
+      <c r="F2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="6" t="n">
         <v>45346</v>
       </c>
-      <c r="H2" s="5" t="n">
+      <c r="I2" s="7" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="J2" s="8" t="n">
+        <v>0.783333333333333</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="16.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="A3" s="3" t="n">
+        <v>42522.5673611111</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="C3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="4" t="n">
         <v>99</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="4" t="n">
+      <c r="F3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="6" t="n">
         <v>42522</v>
       </c>
-      <c r="H3" s="5" t="n">
+      <c r="I3" s="7" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
+      </c>
+      <c r="J3" s="8" t="n">
+        <v>0.0576388888888889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>